<commit_message>
Added HW9 - Done
</commit_message>
<xml_diff>
--- a/Week 9 - Project Cost Budgeting/homework/Wk 8 HB Bill of Materials.xlsx
+++ b/Week 9 - Project Cost Budgeting/homework/Wk 8 HB Bill of Materials.xlsx
@@ -263,7 +263,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -282,6 +282,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -423,7 +429,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -493,6 +499,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -809,10 +821,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -823,10 +835,11 @@
     <col min="4" max="4" width="10.85546875" style="7" customWidth="1"/>
     <col min="5" max="5" width="31.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="4"/>
+    <col min="7" max="7" width="10.42578125" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -835,10 +848,10 @@
       <c r="D1" s="3"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
     </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>1</v>
       </c>
@@ -848,7 +861,7 @@
       <c r="E3" s="22"/>
       <c r="F3" s="23"/>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
@@ -868,7 +881,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="13" t="s">
         <v>8</v>
@@ -880,9 +893,15 @@
         <v>7500</v>
       </c>
       <c r="E5" s="13"/>
-      <c r="F5" s="15"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="15">
+        <v>7000</v>
+      </c>
+      <c r="G5" s="24">
+        <f>D5-F5</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="13" t="s">
         <v>9</v>
@@ -895,8 +914,12 @@
         <v>11</v>
       </c>
       <c r="F6" s="15"/>
-    </row>
-    <row r="7" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="G6" s="24">
+        <f>D6-F6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="13" t="s">
         <v>12</v>
@@ -910,9 +933,15 @@
       <c r="E7" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="15"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="15">
+        <v>2000</v>
+      </c>
+      <c r="G7" s="24">
+        <f>D7-F7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="13" t="s">
         <v>15</v>
@@ -922,9 +951,15 @@
         <v>10000</v>
       </c>
       <c r="E8" s="13"/>
-      <c r="F8" s="15"/>
-    </row>
-    <row r="9" spans="1:6" ht="51" x14ac:dyDescent="0.25">
+      <c r="F8" s="15">
+        <v>10000</v>
+      </c>
+      <c r="G8" s="24">
+        <f>D8-F8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="13" t="s">
         <v>16</v>
@@ -940,7 +975,7 @@
       </c>
       <c r="F9" s="15"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="13" t="s">
         <v>19</v>
@@ -952,9 +987,15 @@
         <v>47200</v>
       </c>
       <c r="E10" s="13"/>
-      <c r="F10" s="16"/>
-    </row>
-    <row r="11" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F10" s="16">
+        <v>47000</v>
+      </c>
+      <c r="G10" s="24">
+        <f>D10-F10</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="13" t="s">
         <v>21</v>
@@ -968,9 +1009,12 @@
       <c r="E11" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="16"/>
-    </row>
-    <row r="12" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F11" s="16">
+        <v>3000</v>
+      </c>
+      <c r="G11" s="24"/>
+    </row>
+    <row r="12" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="13" t="s">
         <v>23</v>
@@ -984,7 +1028,7 @@
       </c>
       <c r="F12" s="15"/>
     </row>
-    <row r="13" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="13" t="s">
         <v>26</v>
@@ -996,11 +1040,17 @@
       <c r="E13" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="16"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13" s="16">
+        <v>14000</v>
+      </c>
+      <c r="G13" s="24">
+        <f>D13-F13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="25" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="13"/>
@@ -1008,9 +1058,15 @@
         <v>1550</v>
       </c>
       <c r="E14" s="13"/>
-      <c r="F14" s="15"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14" s="15">
+        <v>1550</v>
+      </c>
+      <c r="G14" s="24">
+        <f>D14-F14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="13" t="s">
         <v>29</v>
@@ -1020,9 +1076,15 @@
         <v>5200</v>
       </c>
       <c r="E15" s="13"/>
-      <c r="F15" s="16"/>
-    </row>
-    <row r="16" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="F15" s="16">
+        <v>5190</v>
+      </c>
+      <c r="G15" s="24">
+        <f>D15-F15</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="13" t="s">
         <v>30</v>
@@ -1036,9 +1098,15 @@
       <c r="E16" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="15"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16" s="15">
+        <v>2500</v>
+      </c>
+      <c r="G16" s="24">
+        <f>D16-F16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="13" t="s">
         <v>33</v>
@@ -1048,9 +1116,15 @@
         <v>2200</v>
       </c>
       <c r="E17" s="13"/>
-      <c r="F17" s="15"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="15">
+        <v>2200</v>
+      </c>
+      <c r="G17" s="24">
+        <f>D17-F17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="13" t="s">
         <v>34</v>
@@ -1064,9 +1138,15 @@
       <c r="E18" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="F18" s="15"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="15">
+        <v>25000</v>
+      </c>
+      <c r="G18" s="24">
+        <f>D18-F18</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="13" t="s">
         <v>37</v>
@@ -1080,9 +1160,15 @@
       <c r="E19" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F19" s="15"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="15">
+        <v>800</v>
+      </c>
+      <c r="G19" s="24">
+        <f>D19-F19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="13" t="s">
         <v>40</v>
@@ -1094,9 +1180,15 @@
       <c r="E20" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F20" s="16"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="16">
+        <v>12000</v>
+      </c>
+      <c r="G20" s="24">
+        <f>D20-F20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" s="13" t="s">
         <v>42</v>
@@ -1108,11 +1200,17 @@
         <v>3400</v>
       </c>
       <c r="E21" s="13"/>
-      <c r="F21" s="15"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F21" s="15">
+        <v>3400</v>
+      </c>
+      <c r="G21" s="24">
+        <f>D21-F21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="25" t="s">
         <v>43</v>
       </c>
       <c r="C22" s="13" t="s">
@@ -1122,9 +1220,15 @@
         <v>1750</v>
       </c>
       <c r="E22" s="13"/>
-      <c r="F22" s="15"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F22" s="15">
+        <v>1750</v>
+      </c>
+      <c r="G22" s="24">
+        <f>D22-F22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="13" t="s">
         <v>45</v>
@@ -1136,9 +1240,15 @@
         <v>3500</v>
       </c>
       <c r="E23" s="13"/>
-      <c r="F23" s="16"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F23" s="16">
+        <v>3500</v>
+      </c>
+      <c r="G23" s="24">
+        <f>D23-F23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="13" t="s">
         <v>47</v>
@@ -1150,9 +1260,15 @@
         <v>7900</v>
       </c>
       <c r="E24" s="13"/>
-      <c r="F24" s="16"/>
-    </row>
-    <row r="25" spans="1:6" ht="51" x14ac:dyDescent="0.25">
+      <c r="F24" s="16">
+        <v>7900</v>
+      </c>
+      <c r="G24" s="24">
+        <f>D24-F24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="B25" s="13" t="s">
         <v>49</v>
@@ -1166,9 +1282,15 @@
       <c r="E25" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="F25" s="16"/>
-    </row>
-    <row r="26" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="F25" s="16">
+        <v>2400</v>
+      </c>
+      <c r="G25" s="24">
+        <f>D25-F25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
       <c r="B26" s="13" t="s">
         <v>52</v>
@@ -1182,9 +1304,15 @@
       <c r="E26" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="F26" s="15"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F26" s="15">
+        <v>2400</v>
+      </c>
+      <c r="G26" s="24">
+        <f>D26-F26</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="B27" s="13" t="s">
         <v>54</v>
@@ -1198,9 +1326,15 @@
       <c r="E27" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F27" s="15"/>
-    </row>
-    <row r="28" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F27" s="15">
+        <v>12000</v>
+      </c>
+      <c r="G27" s="24">
+        <f>D27-F27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="17" t="s">
         <v>56</v>
       </c>
@@ -1213,7 +1347,7 @@
       <c r="E28" s="18"/>
       <c r="F28" s="20">
         <f>SUM(F5:F27)</f>
-        <v>0</v>
+        <v>165590</v>
       </c>
     </row>
   </sheetData>

</xml_diff>